<commit_message>
More corrections to data modeling and dataset metadata
</commit_message>
<xml_diff>
--- a/data/les-miserables-characters-sdd.xlsx
+++ b/data/les-miserables-characters-sdd.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamie/opt/whyis_census_demo/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3542CF5C-D138-D94A-867E-062FF329E076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BF1F143-DD5A-D94A-9CAF-84DCEEFDD51F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16400" yWindow="8660" windowWidth="35840" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dictionary Mapping" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="55">
   <si>
     <t>Column</t>
   </si>
@@ -199,6 +199,9 @@
   </si>
   <si>
     <t>dcterms</t>
+  </si>
+  <si>
+    <t>person/{id}</t>
   </si>
 </sst>
 </file>
@@ -589,9 +592,9 @@
   </sheetPr>
   <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView zoomScale="241" zoomScaleNormal="241" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" zoomScale="241" zoomScaleNormal="241" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -679,7 +682,9 @@
       <c r="L2" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="R2" s="11"/>
+      <c r="R2" s="11" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="3" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="12" t="s">
@@ -895,7 +900,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E2A108F-5264-9442-8FE9-E0785C39EE7A}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="216" zoomScaleNormal="216" workbookViewId="0">
+    <sheetView zoomScale="216" zoomScaleNormal="216" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added types to missing codebook types.
</commit_message>
<xml_diff>
--- a/data/les-miserables-characters-sdd.xlsx
+++ b/data/les-miserables-characters-sdd.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="456">
   <si>
     <t xml:space="preserve">Column</t>
   </si>
@@ -1699,7 +1699,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="G8" activeCellId="0" sqref="G8"/>
+      <selection pane="topRight" activeCell="G8" activeCellId="1" sqref="D23:D181 G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1856,15 +1856,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
+  <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D133" activeCellId="0" sqref="D133"/>
+      <selection pane="bottomLeft" activeCell="D23" activeCellId="0" sqref="D23:D181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1893,7 +1893,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>18</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>person/AA</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>18</v>
       </c>
@@ -1930,7 +1930,7 @@
       </c>
       <c r="F3" s="9"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>18</v>
       </c>
@@ -1947,7 +1947,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>18</v>
       </c>
@@ -1965,7 +1965,7 @@
         <v>person/BA</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>18</v>
       </c>
@@ -1983,7 +1983,7 @@
         <v>person/BB</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>18</v>
       </c>
@@ -2001,7 +2001,7 @@
         <v>person/BC</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>18</v>
       </c>
@@ -2019,7 +2019,7 @@
         <v>person/BF</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>18</v>
       </c>
@@ -2037,7 +2037,7 @@
         <v>person/BG</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>18</v>
       </c>
@@ -2055,7 +2055,7 @@
         <v>person/BH</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>18</v>
       </c>
@@ -2073,7 +2073,7 @@
         <v>person/BI</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>18</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>18</v>
       </c>
@@ -2108,7 +2108,7 @@
         <v>person/BK</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>18</v>
       </c>
@@ -2126,7 +2126,7 @@
         <v>person/BL</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>18</v>
       </c>
@@ -2143,7 +2143,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>18</v>
       </c>
@@ -2161,7 +2161,7 @@
         <v>person/BO</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>18</v>
       </c>
@@ -2170,13 +2170,16 @@
       </c>
       <c r="C17" s="0" t="s">
         <v>69</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>19</v>
       </c>
       <c r="E17" s="0" t="str">
         <f aca="false">"person/"&amp;B17</f>
         <v>person/BQ</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>18</v>
       </c>
@@ -2194,7 +2197,7 @@
         <v>person/BR</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>18</v>
       </c>
@@ -2212,7 +2215,7 @@
         <v>person/BS</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>18</v>
       </c>
@@ -2230,7 +2233,7 @@
         <v>person/BT</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>18</v>
       </c>
@@ -2248,7 +2251,7 @@
         <v>person/BU</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>18</v>
       </c>
@@ -2276,6 +2279,9 @@
       <c r="C23" s="0" t="s">
         <v>83</v>
       </c>
+      <c r="D23" s="0" t="s">
+        <v>19</v>
+      </c>
       <c r="E23" s="0" t="str">
         <f aca="false">"person/"&amp;B23</f>
         <v>person/BX</v>
@@ -2291,6 +2297,9 @@
       <c r="C24" s="0" t="s">
         <v>85</v>
       </c>
+      <c r="D24" s="0" t="s">
+        <v>19</v>
+      </c>
       <c r="E24" s="0" t="str">
         <f aca="false">"person/"&amp;B24</f>
         <v>person/BY</v>
@@ -2306,12 +2315,15 @@
       <c r="C25" s="0" t="s">
         <v>87</v>
       </c>
+      <c r="D25" s="0" t="s">
+        <v>19</v>
+      </c>
       <c r="E25" s="0" t="str">
         <f aca="false">"person/"&amp;B25</f>
         <v>person/BZ</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>18</v>
       </c>
@@ -2339,12 +2351,15 @@
       <c r="C27" s="0" t="s">
         <v>91</v>
       </c>
+      <c r="D27" s="0" t="s">
+        <v>19</v>
+      </c>
       <c r="E27" s="0" t="str">
         <f aca="false">"person/"&amp;B27</f>
         <v>person/CB</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
         <v>18</v>
       </c>
@@ -2362,7 +2377,7 @@
         <v>person/CC</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>18</v>
       </c>
@@ -2380,7 +2395,7 @@
         <v>person/CD</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>18</v>
       </c>
@@ -2398,7 +2413,7 @@
         <v>person/CE</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>18</v>
       </c>
@@ -2416,7 +2431,7 @@
         <v>person/CF</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>18</v>
       </c>
@@ -2434,7 +2449,7 @@
         <v>person/CG</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>18</v>
       </c>
@@ -2451,7 +2466,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>18</v>
       </c>
@@ -2469,7 +2484,7 @@
         <v>person/CI</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>18</v>
       </c>
@@ -2487,7 +2502,7 @@
         <v>person/CJ</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>18</v>
       </c>
@@ -2505,7 +2520,7 @@
         <v>person/CK</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>18</v>
       </c>
@@ -2523,7 +2538,7 @@
         <v>person/CL</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>18</v>
       </c>
@@ -2540,7 +2555,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
         <v>18</v>
       </c>
@@ -2558,7 +2573,7 @@
         <v>person/CN</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>18</v>
       </c>
@@ -2584,13 +2599,16 @@
       </c>
       <c r="C41" s="0" t="s">
         <v>122</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>19</v>
       </c>
       <c r="E41" s="0" t="str">
         <f aca="false">"person/"&amp;B41</f>
         <v>person/CP</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>18</v>
       </c>
@@ -2616,13 +2634,16 @@
       </c>
       <c r="C43" s="0" t="s">
         <v>127</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>19</v>
       </c>
       <c r="E43" s="0" t="str">
         <f aca="false">"person/"&amp;B43</f>
         <v>person/CV</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>18</v>
       </c>
@@ -2640,7 +2661,7 @@
         <v>person/CW</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
         <v>18</v>
       </c>
@@ -2658,7 +2679,7 @@
         <v>person/CX</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
         <v>18</v>
       </c>
@@ -2676,7 +2697,7 @@
         <v>person/CY</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
         <v>18</v>
       </c>
@@ -2694,7 +2715,7 @@
         <v>person/CZ</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
         <v>18</v>
       </c>
@@ -2712,7 +2733,7 @@
         <v>person/DA</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
         <v>18</v>
       </c>
@@ -2730,7 +2751,7 @@
         <v>person/DG</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
         <v>18</v>
       </c>
@@ -2748,7 +2769,7 @@
         <v>person/DH</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
         <v>18</v>
       </c>
@@ -2766,7 +2787,7 @@
         <v>person/DJ</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
         <v>18</v>
       </c>
@@ -2794,12 +2815,15 @@
       <c r="C53" s="0" t="s">
         <v>150</v>
       </c>
+      <c r="D53" s="0" t="s">
+        <v>19</v>
+      </c>
       <c r="E53" s="0" t="str">
         <f aca="false">"person/"&amp;B53</f>
         <v>person/DN</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
         <v>18</v>
       </c>
@@ -2817,7 +2841,7 @@
         <v>person/DO</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
         <v>18</v>
       </c>
@@ -2835,7 +2859,7 @@
         <v>person/DR</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
         <v>18</v>
       </c>
@@ -2863,12 +2887,15 @@
       <c r="C57" s="0" t="s">
         <v>158</v>
       </c>
+      <c r="D57" s="0" t="s">
+        <v>19</v>
+      </c>
       <c r="E57" s="0" t="str">
         <f aca="false">"person/"&amp;B57</f>
         <v>person/DU</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
         <v>18</v>
       </c>
@@ -2886,7 +2913,7 @@
         <v>person/DV</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
         <v>18</v>
       </c>
@@ -2903,7 +2930,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
         <v>18</v>
       </c>
@@ -2920,7 +2947,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
         <v>18</v>
       </c>
@@ -2938,7 +2965,7 @@
         <v>person/FA</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
         <v>18</v>
       </c>
@@ -2956,7 +2983,7 @@
         <v>person/FB</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
         <v>18</v>
       </c>
@@ -2974,7 +3001,7 @@
         <v>person/FD</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
         <v>18</v>
       </c>
@@ -3001,6 +3028,9 @@
       <c r="C65" s="0" t="s">
         <v>177</v>
       </c>
+      <c r="D65" s="0" t="s">
+        <v>19</v>
+      </c>
       <c r="E65" s="0" t="s">
         <v>178</v>
       </c>
@@ -3014,13 +3044,16 @@
       </c>
       <c r="C66" s="0" t="s">
         <v>180</v>
+      </c>
+      <c r="D66" s="0" t="s">
+        <v>19</v>
       </c>
       <c r="E66" s="0" t="str">
         <f aca="false">"person/"&amp;B66</f>
         <v>person/FL</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
         <v>18</v>
       </c>
@@ -3038,7 +3071,7 @@
         <v>person/FM</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
         <v>18</v>
       </c>
@@ -3055,7 +3088,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
         <v>18</v>
       </c>
@@ -3073,7 +3106,7 @@
         <v>person/FT</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
         <v>18</v>
       </c>
@@ -3091,7 +3124,7 @@
         <v>person/FV</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
         <v>18</v>
       </c>
@@ -3117,13 +3150,16 @@
       </c>
       <c r="C72" s="0" t="s">
         <v>194</v>
+      </c>
+      <c r="D72" s="0" t="s">
+        <v>19</v>
       </c>
       <c r="E72" s="0" t="str">
         <f aca="false">"person/"&amp;B72</f>
         <v>person/GB</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
         <v>18</v>
       </c>
@@ -3151,12 +3187,15 @@
       <c r="C74" s="0" t="s">
         <v>198</v>
       </c>
+      <c r="D74" s="0" t="s">
+        <v>19</v>
+      </c>
       <c r="E74" s="0" t="str">
         <f aca="false">"person/"&amp;B74</f>
         <v>person/GE</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
         <v>18</v>
       </c>
@@ -3184,12 +3223,15 @@
       <c r="C76" s="0" t="s">
         <v>202</v>
       </c>
+      <c r="D76" s="0" t="s">
+        <v>19</v>
+      </c>
       <c r="E76" s="0" t="str">
         <f aca="false">"person/"&amp;B76</f>
         <v>person/GG</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
         <v>18</v>
       </c>
@@ -3217,12 +3259,15 @@
       <c r="C78" s="0" t="s">
         <v>206</v>
       </c>
+      <c r="D78" s="0" t="s">
+        <v>19</v>
+      </c>
       <c r="E78" s="0" t="str">
         <f aca="false">"person/"&amp;B78</f>
         <v>person/GL</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
         <v>18</v>
       </c>
@@ -3240,7 +3285,7 @@
         <v>person/GN</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
         <v>18</v>
       </c>
@@ -3268,12 +3313,15 @@
       <c r="C81" s="0" t="s">
         <v>212</v>
       </c>
+      <c r="D81" s="0" t="s">
+        <v>19</v>
+      </c>
       <c r="E81" s="0" t="str">
         <f aca="false">"person/"&amp;B81</f>
         <v>person/GR</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
         <v>18</v>
       </c>
@@ -3291,7 +3339,7 @@
         <v>person/GS</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
         <v>18</v>
       </c>
@@ -3308,7 +3356,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
         <v>18</v>
       </c>
@@ -3326,7 +3374,7 @@
         <v>person/GU</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
         <v>18</v>
       </c>
@@ -3344,7 +3392,7 @@
         <v>person/GV</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
         <v>18</v>
       </c>
@@ -3372,12 +3420,15 @@
       <c r="C87" s="0" t="s">
         <v>226</v>
       </c>
+      <c r="D87" s="0" t="s">
+        <v>19</v>
+      </c>
       <c r="E87" s="0" t="str">
         <f aca="false">"person/"&amp;B87</f>
         <v>person/HL</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
         <v>18</v>
       </c>
@@ -3405,6 +3456,9 @@
       <c r="C89" s="0" t="s">
         <v>230</v>
       </c>
+      <c r="D89" s="0" t="s">
+        <v>19</v>
+      </c>
       <c r="E89" s="0" t="str">
         <f aca="false">"person/"&amp;B89</f>
         <v>person/IK</v>
@@ -3420,12 +3474,15 @@
       <c r="C90" s="0" t="s">
         <v>232</v>
       </c>
+      <c r="D90" s="0" t="s">
+        <v>19</v>
+      </c>
       <c r="E90" s="0" t="str">
         <f aca="false">"person/"&amp;B90</f>
         <v>person/IS</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
         <v>18</v>
       </c>
@@ -3443,7 +3500,7 @@
         <v>person/IW</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
         <v>18</v>
       </c>
@@ -3460,7 +3517,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
         <v>18</v>
       </c>
@@ -3488,6 +3545,9 @@
       <c r="C94" s="0" t="s">
         <v>241</v>
       </c>
+      <c r="D94" s="0" t="s">
+        <v>19</v>
+      </c>
       <c r="E94" s="0" t="str">
         <f aca="false">"person/"&amp;B94</f>
         <v>person/JL</v>
@@ -3503,6 +3563,9 @@
       <c r="C95" s="0" t="s">
         <v>243</v>
       </c>
+      <c r="D95" s="0" t="s">
+        <v>19</v>
+      </c>
       <c r="E95" s="0" t="str">
         <f aca="false">"person/"&amp;B95</f>
         <v>person/JM</v>
@@ -3518,12 +3581,15 @@
       <c r="C96" s="0" t="s">
         <v>245</v>
       </c>
+      <c r="D96" s="0" t="s">
+        <v>19</v>
+      </c>
       <c r="E96" s="0" t="str">
         <f aca="false">"person/"&amp;B96</f>
         <v>person/JN</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
         <v>18</v>
       </c>
@@ -3540,7 +3606,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
         <v>18</v>
       </c>
@@ -3558,7 +3624,7 @@
         <v>person/JP</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
         <v>18</v>
       </c>
@@ -3576,7 +3642,7 @@
         <v>person/JU</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
         <v>18</v>
       </c>
@@ -3593,7 +3659,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
         <v>18</v>
       </c>
@@ -3611,7 +3677,7 @@
         <v>person/KA</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
         <v>18</v>
       </c>
@@ -3629,7 +3695,7 @@
         <v>person/KB</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
         <v>18</v>
       </c>
@@ -3647,7 +3713,7 @@
         <v>person/KD</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
         <v>18</v>
       </c>
@@ -3665,7 +3731,7 @@
         <v>person/KT</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
         <v>18</v>
       </c>
@@ -3683,7 +3749,7 @@
         <v>person/LA</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
         <v>18</v>
       </c>
@@ -3701,7 +3767,7 @@
         <v>person/LI</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
         <v>18</v>
       </c>
@@ -3729,12 +3795,15 @@
       <c r="C108" s="0" t="s">
         <v>272</v>
       </c>
+      <c r="D108" s="0" t="s">
+        <v>19</v>
+      </c>
       <c r="E108" s="0" t="str">
         <f aca="false">"person/"&amp;B108</f>
         <v>person/LP</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
         <v>18</v>
       </c>
@@ -3752,7 +3821,7 @@
         <v>person/LR</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
         <v>18</v>
       </c>
@@ -3778,6 +3847,9 @@
       </c>
       <c r="C111" s="0" t="s">
         <v>279</v>
+      </c>
+      <c r="D111" s="0" t="s">
+        <v>19</v>
       </c>
       <c r="E111" s="0" t="str">
         <f aca="false">"person/"&amp;B111</f>
@@ -3794,6 +3866,9 @@
       <c r="C112" s="0" t="s">
         <v>281</v>
       </c>
+      <c r="D112" s="0" t="s">
+        <v>19</v>
+      </c>
       <c r="E112" s="0" t="str">
         <f aca="false">"person/"&amp;B112</f>
         <v>person/MC</v>
@@ -3809,12 +3884,15 @@
       <c r="C113" s="0" t="s">
         <v>283</v>
       </c>
+      <c r="D113" s="0" t="s">
+        <v>19</v>
+      </c>
       <c r="E113" s="0" t="str">
         <f aca="false">"person/"&amp;B113</f>
         <v>person/MD</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
         <v>18</v>
       </c>
@@ -3842,12 +3920,15 @@
       <c r="C115" s="0" t="s">
         <v>287</v>
       </c>
+      <c r="D115" s="0" t="s">
+        <v>19</v>
+      </c>
       <c r="E115" s="0" t="str">
         <f aca="false">"person/"&amp;B115</f>
         <v>person/MG</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
         <v>18</v>
       </c>
@@ -3865,7 +3946,7 @@
         <v>person/MH</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
         <v>18</v>
       </c>
@@ -3893,12 +3974,15 @@
       <c r="C118" s="0" t="s">
         <v>293</v>
       </c>
+      <c r="D118" s="0" t="s">
+        <v>19</v>
+      </c>
       <c r="E118" s="0" t="str">
         <f aca="false">"person/"&amp;B118</f>
         <v>person/ML</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
         <v>18</v>
       </c>
@@ -3916,7 +4000,7 @@
         <v>person/MM</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
         <v>18</v>
       </c>
@@ -3934,7 +4018,7 @@
         <v>person/MN</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
         <v>18</v>
       </c>
@@ -3951,7 +4035,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
         <v>18</v>
       </c>
@@ -3969,7 +4053,7 @@
         <v>person/MP</v>
       </c>
     </row>
-    <row r="123" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
         <v>18</v>
       </c>
@@ -3987,7 +4071,7 @@
         <v>person/MR</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
         <v>18</v>
       </c>
@@ -4005,7 +4089,7 @@
         <v>person/MS</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
         <v>18</v>
       </c>
@@ -4023,7 +4107,7 @@
         <v>person/MT</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
         <v>18</v>
       </c>
@@ -4051,6 +4135,9 @@
       <c r="C127" s="0" t="s">
         <v>312</v>
       </c>
+      <c r="D127" s="0" t="s">
+        <v>19</v>
+      </c>
       <c r="E127" s="0" t="str">
         <f aca="false">"person/"&amp;B127</f>
         <v>person/MV</v>
@@ -4066,12 +4153,15 @@
       <c r="C128" s="0" t="s">
         <v>314</v>
       </c>
+      <c r="D128" s="0" t="s">
+        <v>19</v>
+      </c>
       <c r="E128" s="0" t="str">
         <f aca="false">"person/"&amp;B128</f>
         <v>person/MW</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
         <v>18</v>
       </c>
@@ -4097,6 +4187,9 @@
       </c>
       <c r="C130" s="0" t="s">
         <v>319</v>
+      </c>
+      <c r="D130" s="0" t="s">
+        <v>19</v>
       </c>
       <c r="E130" s="0" t="str">
         <f aca="false">"person/"&amp;B130</f>
@@ -4113,12 +4206,15 @@
       <c r="C131" s="0" t="s">
         <v>321</v>
       </c>
+      <c r="D131" s="0" t="s">
+        <v>19</v>
+      </c>
       <c r="E131" s="0" t="str">
         <f aca="false">"person/"&amp;B131</f>
         <v>person/NI</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
         <v>18</v>
       </c>
@@ -4144,13 +4240,16 @@
       </c>
       <c r="C133" s="0" t="s">
         <v>326</v>
+      </c>
+      <c r="D133" s="0" t="s">
+        <v>19</v>
       </c>
       <c r="E133" s="0" t="str">
         <f aca="false">"person/"&amp;B133</f>
         <v>person/NT</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
         <v>18</v>
       </c>
@@ -4168,7 +4267,7 @@
         <v>person/OS</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
         <v>18</v>
       </c>
@@ -4196,12 +4295,15 @@
       <c r="C136" s="0" t="s">
         <v>332</v>
       </c>
+      <c r="D136" s="0" t="s">
+        <v>19</v>
+      </c>
       <c r="E136" s="0" t="str">
         <f aca="false">"person/"&amp;B136</f>
         <v>person/PC</v>
       </c>
     </row>
-    <row r="137" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="137" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
         <v>18</v>
       </c>
@@ -4219,7 +4321,7 @@
         <v>person/PD</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="138" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
         <v>18</v>
       </c>
@@ -4247,12 +4349,15 @@
       <c r="C139" s="0" t="s">
         <v>338</v>
       </c>
+      <c r="D139" s="0" t="s">
+        <v>19</v>
+      </c>
       <c r="E139" s="0" t="str">
         <f aca="false">"person/"&amp;B139</f>
         <v>person/PG</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
         <v>18</v>
       </c>
@@ -4270,7 +4375,7 @@
         <v>person/PH</v>
       </c>
     </row>
-    <row r="141" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
         <v>18</v>
       </c>
@@ -4298,12 +4403,15 @@
       <c r="C142" s="0" t="s">
         <v>344</v>
       </c>
+      <c r="D142" s="0" t="s">
+        <v>19</v>
+      </c>
       <c r="E142" s="0" t="str">
         <f aca="false">"person/"&amp;B142</f>
         <v>person/PN</v>
       </c>
     </row>
-    <row r="143" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="143" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
         <v>18</v>
       </c>
@@ -4321,7 +4429,7 @@
         <v>person/PO</v>
       </c>
     </row>
-    <row r="144" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="144" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
         <v>18</v>
       </c>
@@ -4339,7 +4447,7 @@
         <v>person/PR</v>
       </c>
     </row>
-    <row r="145" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="145" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
         <v>18</v>
       </c>
@@ -4357,7 +4465,7 @@
         <v>person/PS</v>
       </c>
     </row>
-    <row r="146" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="146" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
         <v>18</v>
       </c>
@@ -4375,7 +4483,7 @@
         <v>person/PT</v>
       </c>
     </row>
-    <row r="147" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="147" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
         <v>18</v>
       </c>
@@ -4393,7 +4501,7 @@
         <v>person/PZ</v>
       </c>
     </row>
-    <row r="148" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="148" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
         <v>18</v>
       </c>
@@ -4419,13 +4527,16 @@
       </c>
       <c r="C149" s="0" t="s">
         <v>359</v>
+      </c>
+      <c r="D149" s="0" t="s">
+        <v>19</v>
       </c>
       <c r="E149" s="0" t="str">
         <f aca="false">"person/"&amp;B149</f>
         <v>person/RA</v>
       </c>
     </row>
-    <row r="150" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="150" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
         <v>18</v>
       </c>
@@ -4443,7 +4554,7 @@
         <v>person/RM</v>
       </c>
     </row>
-    <row r="151" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="151" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
         <v>18</v>
       </c>
@@ -4461,7 +4572,7 @@
         <v>person/RP</v>
       </c>
     </row>
-    <row r="152" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="152" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
         <v>18</v>
       </c>
@@ -4489,6 +4600,9 @@
       <c r="C153" s="0" t="s">
         <v>367</v>
       </c>
+      <c r="D153" s="0" t="s">
+        <v>19</v>
+      </c>
       <c r="E153" s="0" t="str">
         <f aca="false">"person/"&amp;B153</f>
         <v>person/SC</v>
@@ -4504,12 +4618,15 @@
       <c r="C154" s="0" t="s">
         <v>369</v>
       </c>
+      <c r="D154" s="0" t="s">
+        <v>19</v>
+      </c>
       <c r="E154" s="0" t="str">
         <f aca="false">"person/"&amp;B154</f>
         <v>person/SD</v>
       </c>
     </row>
-    <row r="155" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="155" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
         <v>18</v>
       </c>
@@ -4527,7 +4644,7 @@
         <v>person/SE</v>
       </c>
     </row>
-    <row r="156" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="156" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
         <v>18</v>
       </c>
@@ -4545,7 +4662,7 @@
         <v>person/SF</v>
       </c>
     </row>
-    <row r="157" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="157" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
         <v>18</v>
       </c>
@@ -4563,7 +4680,7 @@
         <v>person/SG</v>
       </c>
     </row>
-    <row r="158" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="158" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
         <v>18</v>
       </c>
@@ -4581,7 +4698,7 @@
         <v>person/SI</v>
       </c>
     </row>
-    <row r="159" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="159" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
         <v>18</v>
       </c>
@@ -4599,7 +4716,7 @@
         <v>person/SM</v>
       </c>
     </row>
-    <row r="160" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="160" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
         <v>18</v>
       </c>
@@ -4617,7 +4734,7 @@
         <v>person/SN</v>
       </c>
     </row>
-    <row r="161" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="161" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
         <v>18</v>
       </c>
@@ -4635,7 +4752,7 @@
         <v>person/SO</v>
       </c>
     </row>
-    <row r="162" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="162" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
         <v>18</v>
       </c>
@@ -4653,7 +4770,7 @@
         <v>person/SP</v>
       </c>
     </row>
-    <row r="163" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="163" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
         <v>18</v>
       </c>
@@ -4671,7 +4788,7 @@
         <v>person/SR</v>
       </c>
     </row>
-    <row r="164" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="164" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
         <v>18</v>
       </c>
@@ -4689,7 +4806,7 @@
         <v>person/SS</v>
       </c>
     </row>
-    <row r="165" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="165" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
         <v>18</v>
       </c>
@@ -4707,7 +4824,7 @@
         <v>person/SW</v>
       </c>
     </row>
-    <row r="166" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="166" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
         <v>18</v>
       </c>
@@ -4725,7 +4842,7 @@
         <v>person/TC</v>
       </c>
     </row>
-    <row r="167" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="167" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
         <v>18</v>
       </c>
@@ -4743,7 +4860,7 @@
         <v>person/TE</v>
       </c>
     </row>
-    <row r="168" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="168" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
         <v>18</v>
       </c>
@@ -4761,7 +4878,7 @@
         <v>person/TG</v>
       </c>
     </row>
-    <row r="169" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="169" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
         <v>18</v>
       </c>
@@ -4778,7 +4895,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="170" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="170" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
         <v>18</v>
       </c>
@@ -4795,7 +4912,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="171" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="171" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
         <v>18</v>
       </c>
@@ -4813,7 +4930,7 @@
         <v>person/TR</v>
       </c>
     </row>
-    <row r="172" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="172" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
         <v>18</v>
       </c>
@@ -4841,6 +4958,9 @@
       <c r="C173" s="0" t="s">
         <v>409</v>
       </c>
+      <c r="D173" s="0" t="s">
+        <v>19</v>
+      </c>
       <c r="E173" s="0" t="str">
         <f aca="false">"person/"&amp;B173</f>
         <v>person/VB</v>
@@ -4856,12 +4976,15 @@
       <c r="C174" s="0" t="s">
         <v>411</v>
       </c>
+      <c r="D174" s="0" t="s">
+        <v>19</v>
+      </c>
       <c r="E174" s="0" t="str">
         <f aca="false">"person/"&amp;B174</f>
         <v>person/VI</v>
       </c>
     </row>
-    <row r="175" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="175" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
         <v>18</v>
       </c>
@@ -4879,7 +5002,7 @@
         <v>person/WA</v>
       </c>
     </row>
-    <row r="176" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="176" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
         <v>18</v>
       </c>
@@ -4907,6 +5030,9 @@
       <c r="C177" s="0" t="s">
         <v>417</v>
       </c>
+      <c r="D177" s="0" t="s">
+        <v>19</v>
+      </c>
       <c r="E177" s="0" t="str">
         <f aca="false">"person/"&amp;B177</f>
         <v>person/WH</v>
@@ -4922,12 +5048,15 @@
       <c r="C178" s="0" t="s">
         <v>419</v>
       </c>
+      <c r="D178" s="0" t="s">
+        <v>19</v>
+      </c>
       <c r="E178" s="0" t="str">
         <f aca="false">"person/"&amp;B178</f>
         <v>person/WI</v>
       </c>
     </row>
-    <row r="179" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="179" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
         <v>18</v>
       </c>
@@ -4955,6 +5084,9 @@
       <c r="C180" s="0" t="s">
         <v>423</v>
       </c>
+      <c r="D180" s="0" t="s">
+        <v>19</v>
+      </c>
       <c r="E180" s="0" t="str">
         <f aca="false">"person/"&amp;B180</f>
         <v>person/XA</v>
@@ -4970,12 +5102,15 @@
       <c r="C181" s="0" t="s">
         <v>425</v>
       </c>
+      <c r="D181" s="0" t="s">
+        <v>19</v>
+      </c>
       <c r="E181" s="0" t="str">
         <f aca="false">"person/"&amp;B181</f>
         <v>person/XB</v>
       </c>
     </row>
-    <row r="182" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="182" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
         <v>18</v>
       </c>
@@ -4995,7 +5130,11 @@
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A1:E182"/>
+  <autoFilter ref="A1:E182">
+    <filterColumn colId="3">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -5015,7 +5154,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D23:D181 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5090,7 +5229,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="1" sqref="D23:D181 B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5163,7 +5302,7 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D23:D181 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5198,7 +5337,7 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D23:D181 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>